<commit_message>
UR Table dimensions added
Tout est dans le titre
</commit_message>
<xml_diff>
--- a/doc/dimensions.xlsx
+++ b/doc/dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André\Documents\MyKHIlibraries\Projects\SandBox\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5068D677-3474-4727-BF77-005CC743BE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78C4018-0528-4D98-B595-DCE416426B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-225" yWindow="16680" windowWidth="29040" windowHeight="15840" xr2:uid="{8245ACA6-7B8B-412B-B24A-3DB3ED4B8A06}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8245ACA6-7B8B-412B-B24A-3DB3ED4B8A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Object</t>
   </si>
@@ -50,13 +50,19 @@
     <t>Box</t>
   </si>
   <si>
-    <t>X (cm)</t>
-  </si>
-  <si>
-    <t>Y (cm)</t>
-  </si>
-  <si>
-    <t>Z (cm)</t>
+    <t>Table UR</t>
+  </si>
+  <si>
+    <t>Support UR</t>
+  </si>
+  <si>
+    <t>Z (mm)</t>
+  </si>
+  <si>
+    <t>Y (mm)</t>
+  </si>
+  <si>
+    <t>X (mm)</t>
   </si>
 </sst>
 </file>
@@ -112,13 +118,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A1D1B8B-B9C0-4DD8-A3C9-8F450676F381}" name="Tableau1" displayName="Tableau1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{4A1D1B8B-B9C0-4DD8-A3C9-8F450676F381}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A1D1B8B-B9C0-4DD8-A3C9-8F450676F381}" name="Tableau1" displayName="Tableau1" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{4A1D1B8B-B9C0-4DD8-A3C9-8F450676F381}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{81709E10-B352-432A-AEB0-D475FBBA66DC}" name="Object"/>
-    <tableColumn id="2" xr3:uid="{7C5F5647-085F-401F-B13A-D07743581B6C}" name="X (cm)"/>
-    <tableColumn id="3" xr3:uid="{72754A8A-6223-41D7-9AF9-C2D628A908E7}" name="Y (cm)"/>
-    <tableColumn id="4" xr3:uid="{33384F3E-11FE-43DB-AF92-3A7FA4845558}" name="Z (cm)"/>
+    <tableColumn id="2" xr3:uid="{7C5F5647-085F-401F-B13A-D07743581B6C}" name="X (mm)"/>
+    <tableColumn id="3" xr3:uid="{72754A8A-6223-41D7-9AF9-C2D628A908E7}" name="Y (mm)"/>
+    <tableColumn id="4" xr3:uid="{33384F3E-11FE-43DB-AF92-3A7FA4845558}" name="Z (mm)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,68 +427,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A102DF-63FC-44FA-8AC6-6CB571730C80}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="C2">
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>2.5</v>
-      </c>
-      <c r="D3">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="C4">
-        <v>22.5</v>
+        <v>225</v>
       </c>
       <c r="D4">
-        <v>10.5</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>870</v>
+      </c>
+      <c r="C5">
+        <v>580</v>
+      </c>
+      <c r="D5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added size of parts and station
</commit_message>
<xml_diff>
--- a/doc/dimensions.xlsx
+++ b/doc/dimensions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathj\OneDrive\Documents\GitHub\Internship\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78C4018-0528-4D98-B595-DCE416426B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C83103-71B0-4CC7-B90F-5F5FDE8D77BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8245ACA6-7B8B-412B-B24A-3DB3ED4B8A06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8245ACA6-7B8B-412B-B24A-3DB3ED4B8A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Object</t>
   </si>
@@ -63,13 +63,28 @@
   </si>
   <si>
     <t>X (mm)</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>P Station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,16 +92,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,12 +129,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A102DF-63FC-44FA-8AC6-6CB571730C80}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +501,14 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,8 +521,14 @@
       <c r="D2">
         <v>30</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -476,8 +541,14 @@
       <c r="D3">
         <v>15</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -491,7 +562,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -504,8 +575,14 @@
       <c r="D5">
         <v>28</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -517,12 +594,19 @@
       </c>
       <c r="D6">
         <v>40</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>